<commit_message>
Add ECG and update identifiers to use OIDs
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.condition.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.condition.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.5-beta</t>
+    <t>0.1.6-beta</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-05T12:38:40-06:00</t>
+    <t>2023-03-23T11:34:13-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -707,7 +707,7 @@
     <t>FiveWs.identifier</t>
   </si>
   <si>
-    <t>{StationNbr} | `;` | {ProblemTO.id}</t>
+    <t>{StationNbr} and {ProblemTO.id}</t>
   </si>
   <si>
     <t>Condition.identifier:TOid</t>
@@ -804,7 +804,7 @@
     <t>Condition.identifier.system</t>
   </si>
   <si>
-    <t>The namespace for the identifier value</t>
+    <t>urn:oid:2.16.840.1.113883.4.349.4.{stationNbr}</t>
   </si>
   <si>
     <t>Establishes the namespace for the value - that is, a URL that describes a set values that are unique.</t>
@@ -816,9 +816,6 @@
     <t>There are many sets  of identifiers.  To perform matching of two identifiers, we need to know what set we're dealing with. The system identifies a particular set of unique identifiers.</t>
   </si>
   <si>
-    <t>urn:oid:2.16.840.1.113883.4.349</t>
-  </si>
-  <si>
     <t>http://www.acme.com/identifiers/patient</t>
   </si>
   <si>
@@ -835,6 +832,9 @@
   </si>
   <si>
     <t>Condition.identifier.value</t>
+  </si>
+  <si>
+    <t>`ProblemTO` | `.` | {ProblemTO.id}</t>
   </si>
   <si>
     <t>The portion of the identifier typically relevant to the user and which is unique within the context of the system.</t>
@@ -4461,7 +4461,7 @@
         <v>92</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>80</v>
@@ -5114,46 +5114,46 @@
         <v>80</v>
       </c>
       <c r="S26" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T26" t="s" s="2">
         <v>255</v>
       </c>
-      <c r="T26" t="s" s="2">
+      <c r="U26" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V26" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W26" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X26" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y26" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z26" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA26" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB26" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC26" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD26" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE26" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF26" t="s" s="2">
         <v>256</v>
-      </c>
-      <c r="U26" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="V26" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="W26" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="X26" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="Y26" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="Z26" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AA26" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AB26" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AC26" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AD26" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AE26" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AF26" t="s" s="2">
-        <v>257</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>81</v>
@@ -5174,10 +5174,10 @@
         <v>80</v>
       </c>
       <c r="AM26" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="AN26" t="s" s="2">
         <v>258</v>
-      </c>
-      <c r="AN26" t="s" s="2">
-        <v>259</v>
       </c>
       <c r="AO26" t="s" s="2">
         <v>80</v>
@@ -5191,10 +5191,10 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="B27" t="s" s="2">
         <v>260</v>
-      </c>
-      <c r="B27" t="s" s="2">
-        <v>261</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -5220,7 +5220,7 @@
         <v>106</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>219</v>
+        <v>261</v>
       </c>
       <c r="M27" t="s" s="2">
         <v>262</v>

</xml_diff>

<commit_message>
add API details for Condition
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.PHR.condition.xlsx
+++ b/docs/StructureDefinition-VA.MHV.PHR.condition.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2486" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2486" uniqueCount="464">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-06-13T11:38:47-05:00</t>
+    <t>2023-06-13T14:37:26-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -84,15 +84,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>A profile on the Condition resource for MHV PHR exposing Problems using FHIR API.
-- The mock example maps best to VIA_v4.0.7_uat.wsdl. 
-- Should be based on US-Core for Condition Resource
-- Presume we will not expose those that are ProblemTO.removed = true
-TODO:
-- not clear if the ProblemTO.location is describing, is it evidence?
-- what are the other values for ProblemTO.status
-- not clear what ProblemTO.accuity.tag is
-- not clear what ProblemTo.facility is</t>
+    <t>A profile on the Condition resource for MHV PHR exposing Problems using FHIR API.</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -791,6 +783,14 @@
     <t>The data type is CodeableConcept because clinicalStatus has some clinical judgment involved, such that there might need to be more specificity than the required FHIR value set allows. For example, a SNOMED coding might allow for additional specificity.</t>
   </si>
   <si>
+    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
+  &lt;coding&gt;
+    &lt;system value="http://terminology.hl7.org/CodeSystem/condition-clinical"/&gt;
+    &lt;code value="active"/&gt;
+  &lt;/coding&gt;
+&lt;/valueCodeableConcept&gt;</t>
+  </si>
+  <si>
     <t>http://hl7.org/fhir/ValueSet/condition-clinical</t>
   </si>
   <si>
@@ -814,7 +814,7 @@
     <t>FiveWs.status</t>
   </si>
   <si>
-    <t>ProblemTO.status | !ProblemTO.removed ? `#active` : todo</t>
+    <t>ProblemTO.status==ACTIVE &amp; !ProblemTO.removed ? `#active` : todo</t>
   </si>
   <si>
     <t>Condition.verificationStatus</t>
@@ -830,7 +830,7 @@
 The data type is CodeableConcept because verificationStatus has some clinical judgment involved, such that there might need to be more specificity than the required FHIR value set allows. For example, a SNOMED coding might allow for additional specificity.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/condition-ver-status</t>
+    <t>https://johnmoehrke.github.io/MHV-PHR/ValueSet/ConditionVerificationVS</t>
   </si>
   <si>
     <t>con-3
@@ -863,6 +863,14 @@
   </si>
   <si>
     <t>The categorization is often highly contextual and may appear poorly differentiated or not very useful in other contexts.</t>
+  </si>
+  <si>
+    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
+  &lt;coding&gt;
+    &lt;system value="http://terminology.hl7.org/CodeSystem/condition-category"/&gt;
+    &lt;code value="problem-list-item"/&gt;
+  &lt;/coding&gt;
+&lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/condition-category</t>
@@ -995,64 +1003,64 @@
     <t>246090004</t>
   </si>
   <si>
+    <t>Condition.code.id</t>
+  </si>
+  <si>
+    <t>Condition.code.extension</t>
+  </si>
+  <si>
+    <t>Condition.code.coding</t>
+  </si>
+  <si>
+    <t>Code defined by a terminology system</t>
+  </si>
+  <si>
+    <t>A reference to a code defined by a terminology system.</t>
+  </si>
+  <si>
+    <t>Codes may be defined very casually in enumerations, or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.  Ordering of codings is undefined and SHALL NOT be used to infer meaning. Generally, at most only one of the coding values will be labeled as UserSelected = true.</t>
+  </si>
+  <si>
+    <t>Allows for alternative encodings within a code system, and translations to other code systems.</t>
+  </si>
+  <si>
+    <t>CodeableConcept.coding</t>
+  </si>
+  <si>
+    <t>C*E.1-8, C*E.10-22</t>
+  </si>
+  <si>
+    <t>union(., ./translation)</t>
+  </si>
+  <si>
+    <t>ICD-9 # ProblemTO.icd</t>
+  </si>
+  <si>
+    <t>Condition.code.text</t>
+  </si>
+  <si>
+    <t>Plain text representation of the concept</t>
+  </si>
+  <si>
+    <t>A human language representation of the concept as seen/selected/uttered by the user who entered the data and/or which represents the intended meaning of the user.</t>
+  </si>
+  <si>
+    <t>Very often the text is the same as a displayName of one of the codings.</t>
+  </si>
+  <si>
+    <t>The codes from the terminologies do not always capture the correct meaning with all the nuances of the human using them, or sometimes there is no appropriate code at all. In these cases, the text is used to capture the full meaning of the source.</t>
+  </si>
+  <si>
+    <t>CodeableConcept.text</t>
+  </si>
+  <si>
+    <t>C*E.9. But note many systems use C*E.2 for this</t>
+  </si>
+  <si>
+    <t>./originalText[mediaType/code="text/plain"]/data</t>
+  </si>
+  <si>
     <t>ProblemTO.type.name</t>
-  </si>
-  <si>
-    <t>Condition.code.id</t>
-  </si>
-  <si>
-    <t>Condition.code.extension</t>
-  </si>
-  <si>
-    <t>Condition.code.coding</t>
-  </si>
-  <si>
-    <t>Code defined by a terminology system</t>
-  </si>
-  <si>
-    <t>A reference to a code defined by a terminology system.</t>
-  </si>
-  <si>
-    <t>Codes may be defined very casually in enumerations, or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.  Ordering of codings is undefined and SHALL NOT be used to infer meaning. Generally, at most only one of the coding values will be labeled as UserSelected = true.</t>
-  </si>
-  <si>
-    <t>Allows for alternative encodings within a code system, and translations to other code systems.</t>
-  </si>
-  <si>
-    <t>CodeableConcept.coding</t>
-  </si>
-  <si>
-    <t>C*E.1-8, C*E.10-22</t>
-  </si>
-  <si>
-    <t>union(., ./translation)</t>
-  </si>
-  <si>
-    <t>ICD-9 # ProblemTO.icd</t>
-  </si>
-  <si>
-    <t>Condition.code.text</t>
-  </si>
-  <si>
-    <t>Plain text representation of the concept</t>
-  </si>
-  <si>
-    <t>A human language representation of the concept as seen/selected/uttered by the user who entered the data and/or which represents the intended meaning of the user.</t>
-  </si>
-  <si>
-    <t>Very often the text is the same as a displayName of one of the codings.</t>
-  </si>
-  <si>
-    <t>The codes from the terminologies do not always capture the correct meaning with all the nuances of the human using them, or sometimes there is no appropriate code at all. In these cases, the text is used to capture the full meaning of the source.</t>
-  </si>
-  <si>
-    <t>CodeableConcept.text</t>
-  </si>
-  <si>
-    <t>C*E.9. But note many systems use C*E.2 for this</t>
-  </si>
-  <si>
-    <t>./originalText[mediaType/code="text/plain"]/data</t>
   </si>
   <si>
     <t>Condition.bodySite</t>
@@ -1148,8 +1156,8 @@
     <t>Condition.onset[x]</t>
   </si>
   <si>
-    <t>dateTime
-AgePeriodRangestring</t>
+    <t xml:space="preserve">dateTime
+</t>
   </si>
   <si>
     <t>Estimated or actual date,  date-time, or age</t>
@@ -1165,6 +1173,9 @@
 </t>
   </si>
   <si>
+    <t>closed</t>
+  </si>
+  <si>
     <t>Event.occurrence[x]</t>
   </si>
   <si>
@@ -1181,10 +1192,6 @@
   </si>
   <si>
     <t>onsetDateTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dateTime
-</t>
   </si>
   <si>
     <t>ProblemTO.onsetDate</t>
@@ -1264,6 +1271,10 @@
     <t>Condition.asserter</t>
   </si>
   <si>
+    <t xml:space="preserve">Reference(Practitioner)
+</t>
+  </si>
+  <si>
     <t>Person who asserts this condition</t>
   </si>
   <si>
@@ -1391,10 +1402,6 @@
   </si>
   <si>
     <t>The evidence may be a simple list of coded symptoms/manifestations, or references to observations or formal assessments, or both.</t>
-  </si>
-  <si>
-    <t>con-2:evidence SHALL have code or details {code.exists() or detail.exists()}
-ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}</t>
   </si>
   <si>
     <t>.outboundRelationship[typeCode=SPRT].target[classCode=OBS, moodCode=EVN]</t>
@@ -1835,12 +1842,12 @@
     <col min="23" max="23" width="1.0390625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="10.19140625" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="95.77734375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="66.375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="69.14453125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="1.0390625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="13.390625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="1.0390625" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="5.60546875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="31" max="31" width="6.7421875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="2.15234375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="2.15234375" customWidth="true" bestFit="true"/>
@@ -1852,7 +1859,7 @@
     <col min="40" max="40" width="213.04296875" customWidth="true" bestFit="true"/>
     <col min="41" max="41" width="16.20703125" customWidth="true" bestFit="true"/>
     <col min="42" max="42" width="11.07421875" customWidth="true" bestFit="true"/>
-    <col min="43" max="43" width="54.01171875" customWidth="true" bestFit="true"/>
+    <col min="43" max="43" width="63.0859375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5349,7 +5356,7 @@
         <v>37</v>
       </c>
       <c r="S29" t="s" s="2">
-        <v>37</v>
+        <v>246</v>
       </c>
       <c r="T29" t="s" s="2">
         <v>37</v>
@@ -5368,7 +5375,7 @@
       </c>
       <c r="Y29" s="2"/>
       <c r="Z29" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AA29" t="s" s="2">
         <v>37</v>
@@ -5395,39 +5402,39 @@
         <v>49</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AJ29" t="s" s="2">
         <v>61</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AP29" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AQ29" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5453,13 +5460,13 @@
         <v>197</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
@@ -5489,7 +5496,7 @@
       </c>
       <c r="Y30" s="2"/>
       <c r="Z30" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AA30" t="s" s="2">
         <v>37</v>
@@ -5507,7 +5514,7 @@
         <v>37</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>38</v>
@@ -5516,39 +5523,39 @@
         <v>49</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>61</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AO30" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AP30" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AQ30" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5574,13 +5581,13 @@
         <v>197</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" t="s" s="2">
@@ -5591,7 +5598,7 @@
         <v>37</v>
       </c>
       <c r="S31" t="s" s="2">
-        <v>37</v>
+        <v>270</v>
       </c>
       <c r="T31" t="s" s="2">
         <v>37</v>
@@ -5609,16 +5616,16 @@
         <v>108</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="Z31" t="s" s="2">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="AA31" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AB31" t="s" s="2">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="AC31" s="2"/>
       <c r="AD31" t="s" s="2">
@@ -5628,7 +5635,7 @@
         <v>76</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>38</v>
@@ -5646,33 +5653,33 @@
         <v>37</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="AP31" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AQ31" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C32" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D32" t="s" s="2">
         <v>37</v>
@@ -5697,13 +5704,13 @@
         <v>197</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="O32" s="2"/>
       <c r="P32" t="s" s="2">
@@ -5733,7 +5740,7 @@
       </c>
       <c r="Y32" s="2"/>
       <c r="Z32" t="s" s="2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="AA32" t="s" s="2">
         <v>37</v>
@@ -5751,7 +5758,7 @@
         <v>37</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>38</v>
@@ -5769,16 +5776,16 @@
         <v>37</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="AO32" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="AP32" t="s" s="2">
         <v>37</v>
@@ -5789,13 +5796,13 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C33" t="s" s="2">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D33" t="s" s="2">
         <v>37</v>
@@ -5820,13 +5827,13 @@
         <v>197</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" t="s" s="2">
@@ -5837,7 +5844,7 @@
         <v>37</v>
       </c>
       <c r="S33" t="s" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="T33" t="s" s="2">
         <v>37</v>
@@ -5855,10 +5862,10 @@
         <v>108</v>
       </c>
       <c r="Y33" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="Z33" t="s" s="2">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="AA33" t="s" s="2">
         <v>37</v>
@@ -5876,7 +5883,7 @@
         <v>37</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>38</v>
@@ -5894,16 +5901,16 @@
         <v>37</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="AO33" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="AP33" t="s" s="2">
         <v>37</v>
@@ -5914,10 +5921,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5928,7 +5935,7 @@
         <v>38</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>37</v>
@@ -5943,13 +5950,13 @@
         <v>197</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="O34" s="2"/>
       <c r="P34" t="s" s="2">
@@ -5978,28 +5985,28 @@
         <v>130</v>
       </c>
       <c r="Y34" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="Z34" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="AA34" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB34" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC34" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD34" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE34" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AF34" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="Z34" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="AA34" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB34" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC34" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD34" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE34" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AF34" t="s" s="2">
-        <v>284</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>38</v>
@@ -6017,19 +6024,19 @@
         <v>37</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="AO34" t="s" s="2">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="AP34" t="s" s="2">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="AQ34" t="s" s="2">
         <v>37</v>
@@ -6037,14 +6044,14 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
@@ -6066,14 +6073,14 @@
         <v>197</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="P35" t="s" s="2">
         <v>37</v>
@@ -6101,10 +6108,10 @@
         <v>108</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="Z35" t="s" s="2">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="AA35" t="s" s="2">
         <v>37</v>
@@ -6122,7 +6129,7 @@
         <v>37</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>38</v>
@@ -6137,33 +6144,33 @@
         <v>61</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="AO35" t="s" s="2">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="AP35" t="s" s="2">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="AQ35" t="s" s="2">
-        <v>307</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -6281,10 +6288,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6404,10 +6411,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6433,16 +6440,16 @@
         <v>104</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="O38" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>37</v>
@@ -6491,7 +6498,7 @@
         <v>37</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>38</v>
@@ -6512,10 +6519,10 @@
         <v>37</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AO38" t="s" s="2">
         <v>37</v>
@@ -6524,15 +6531,15 @@
         <v>37</v>
       </c>
       <c r="AQ38" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6558,16 +6565,16 @@
         <v>63</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="O39" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="P39" t="s" s="2">
         <v>37</v>
@@ -6616,7 +6623,7 @@
         <v>37</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>38</v>
@@ -6637,10 +6644,10 @@
         <v>37</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AO39" t="s" s="2">
         <v>37</v>
@@ -6649,15 +6656,15 @@
         <v>37</v>
       </c>
       <c r="AQ39" t="s" s="2">
-        <v>37</v>
+        <v>328</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6668,7 +6675,7 @@
         <v>38</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H40" t="s" s="2">
         <v>37</v>
@@ -6683,13 +6690,13 @@
         <v>197</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="O40" s="2"/>
       <c r="P40" t="s" s="2">
@@ -6718,10 +6725,10 @@
         <v>116</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="Z40" t="s" s="2">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="AA40" t="s" s="2">
         <v>37</v>
@@ -6739,7 +6746,7 @@
         <v>37</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>38</v>
@@ -6757,19 +6764,19 @@
         <v>37</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AN40" t="s" s="2">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="AO40" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AP40" t="s" s="2">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="AQ40" t="s" s="2">
         <v>37</v>
@@ -6777,14 +6784,14 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s" s="2">
@@ -6803,17 +6810,17 @@
         <v>50</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="P41" t="s" s="2">
         <v>37</v>
@@ -6862,7 +6869,7 @@
         <v>37</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>49</v>
@@ -6877,33 +6884,33 @@
         <v>61</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="AO41" t="s" s="2">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="AP41" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AQ41" t="s" s="2">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6914,7 +6921,7 @@
         <v>38</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="H42" t="s" s="2">
         <v>37</v>
@@ -6926,16 +6933,16 @@
         <v>50</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
@@ -6985,7 +6992,7 @@
         <v>37</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>38</v>
@@ -7000,19 +7007,19 @@
         <v>61</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="AO42" t="s" s="2">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="AP42" t="s" s="2">
         <v>37</v>
@@ -7023,10 +7030,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -7049,16 +7056,16 @@
         <v>50</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" t="s" s="2">
@@ -7096,17 +7103,17 @@
         <v>37</v>
       </c>
       <c r="AB43" t="s" s="2">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="AC43" s="2"/>
       <c r="AD43" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>76</v>
+        <v>364</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>38</v>
@@ -7121,19 +7128,19 @@
         <v>61</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="AO43" t="s" s="2">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="AP43" t="s" s="2">
         <v>37</v>
@@ -7144,13 +7151,13 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C44" t="s" s="2">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="D44" t="s" s="2">
         <v>37</v>
@@ -7172,16 +7179,16 @@
         <v>50</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="O44" s="2"/>
       <c r="P44" t="s" s="2">
@@ -7231,7 +7238,7 @@
         <v>37</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>38</v>
@@ -7246,33 +7253,33 @@
         <v>61</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="AO44" t="s" s="2">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="AP44" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AQ44" t="s" s="2">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -7295,16 +7302,16 @@
         <v>37</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
@@ -7342,17 +7349,17 @@
         <v>37</v>
       </c>
       <c r="AB45" t="s" s="2">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="AC45" s="2"/>
       <c r="AD45" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>76</v>
+        <v>364</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>38</v>
@@ -7361,7 +7368,7 @@
         <v>49</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>61</v>
@@ -7376,10 +7383,10 @@
         <v>37</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="AO45" t="s" s="2">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="AP45" t="s" s="2">
         <v>37</v>
@@ -7390,13 +7397,13 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C46" t="s" s="2">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D46" t="s" s="2">
         <v>37</v>
@@ -7418,16 +7425,16 @@
         <v>37</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
@@ -7477,7 +7484,7 @@
         <v>37</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>38</v>
@@ -7486,7 +7493,7 @@
         <v>49</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="AJ46" t="s" s="2">
         <v>61</v>
@@ -7501,24 +7508,24 @@
         <v>37</v>
       </c>
       <c r="AN46" t="s" s="2">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="AO46" t="s" s="2">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="AP46" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AQ46" t="s" s="2">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7541,13 +7548,13 @@
         <v>50</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -7598,7 +7605,7 @@
         <v>37</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>38</v>
@@ -7619,27 +7626,27 @@
         <v>37</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="AN47" t="s" s="2">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="AO47" t="s" s="2">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="AP47" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AQ47" t="s" s="2">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7650,7 +7657,7 @@
         <v>38</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>37</v>
@@ -7662,13 +7669,13 @@
         <v>50</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -7719,7 +7726,7 @@
         <v>37</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>38</v>
@@ -7743,10 +7750,10 @@
         <v>37</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="AO48" t="s" s="2">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="AP48" t="s" s="2">
         <v>37</v>
@@ -7757,10 +7764,10 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7774,7 +7781,7 @@
         <v>49</v>
       </c>
       <c r="H49" t="s" s="2">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="I49" t="s" s="2">
         <v>37</v>
@@ -7783,13 +7790,13 @@
         <v>50</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>388</v>
+        <v>396</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -7840,7 +7847,7 @@
         <v>37</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>38</v>
@@ -7861,27 +7868,27 @@
         <v>37</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="AO49" t="s" s="2">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="AP49" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AQ49" t="s" s="2">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7892,7 +7899,7 @@
         <v>38</v>
       </c>
       <c r="G50" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H50" t="s" s="2">
         <v>37</v>
@@ -7904,13 +7911,13 @@
         <v>37</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -7961,7 +7968,7 @@
         <v>37</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>38</v>
@@ -7973,7 +7980,7 @@
         <v>37</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="AK50" t="s" s="2">
         <v>37</v>
@@ -7985,7 +7992,7 @@
         <v>37</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="AO50" t="s" s="2">
         <v>37</v>
@@ -7999,10 +8006,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -8120,10 +8127,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -8243,14 +8250,14 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" t="s" s="2">
@@ -8272,10 +8279,10 @@
         <v>70</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="N53" t="s" s="2">
         <v>73</v>
@@ -8330,7 +8337,7 @@
         <v>37</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>38</v>
@@ -8368,10 +8375,10 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -8397,10 +8404,10 @@
         <v>197</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
@@ -8430,28 +8437,28 @@
         <v>116</v>
       </c>
       <c r="Y54" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE54" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AF54" t="s" s="2">
         <v>416</v>
-      </c>
-      <c r="Z54" t="s" s="2">
-        <v>417</v>
-      </c>
-      <c r="AA54" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB54" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC54" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD54" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE54" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AF54" t="s" s="2">
-        <v>413</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>38</v>
@@ -8460,7 +8467,7 @@
         <v>49</v>
       </c>
       <c r="AI54" t="s" s="2">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="AJ54" t="s" s="2">
         <v>61</v>
@@ -8469,13 +8476,13 @@
         <v>37</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN54" t="s" s="2">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="AO54" t="s" s="2">
         <v>37</v>
@@ -8489,10 +8496,10 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -8515,13 +8522,13 @@
         <v>37</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -8572,7 +8579,7 @@
         <v>37</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>38</v>
@@ -8581,7 +8588,7 @@
         <v>39</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="AJ55" t="s" s="2">
         <v>61</v>
@@ -8596,7 +8603,7 @@
         <v>37</v>
       </c>
       <c r="AN55" t="s" s="2">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="AO55" t="s" s="2">
         <v>37</v>
@@ -8610,10 +8617,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8639,10 +8646,10 @@
         <v>197</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -8672,28 +8679,28 @@
         <v>116</v>
       </c>
       <c r="Y56" t="s" s="2">
+        <v>431</v>
+      </c>
+      <c r="Z56" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="AA56" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB56" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC56" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD56" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE56" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AF56" t="s" s="2">
         <v>428</v>
-      </c>
-      <c r="Z56" t="s" s="2">
-        <v>429</v>
-      </c>
-      <c r="AA56" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB56" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AC56" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AD56" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AE56" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AF56" t="s" s="2">
-        <v>425</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>38</v>
@@ -8717,7 +8724,7 @@
         <v>37</v>
       </c>
       <c r="AN56" t="s" s="2">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="AO56" t="s" s="2">
         <v>37</v>
@@ -8731,10 +8738,10 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8757,16 +8764,16 @@
         <v>37</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="O57" s="2"/>
       <c r="P57" t="s" s="2">
@@ -8816,7 +8823,7 @@
         <v>37</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>38</v>
@@ -8828,7 +8835,7 @@
         <v>37</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>435</v>
+        <v>37</v>
       </c>
       <c r="AK57" t="s" s="2">
         <v>37</v>
@@ -8840,7 +8847,7 @@
         <v>37</v>
       </c>
       <c r="AN57" t="s" s="2">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="AO57" t="s" s="2">
         <v>37</v>
@@ -8854,10 +8861,10 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8975,10 +8982,10 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -9098,14 +9105,14 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" t="s" s="2">
@@ -9127,10 +9134,10 @@
         <v>70</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="N60" t="s" s="2">
         <v>73</v>
@@ -9185,7 +9192,7 @@
         <v>37</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>38</v>
@@ -9223,10 +9230,10 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -9237,7 +9244,7 @@
         <v>38</v>
       </c>
       <c r="G61" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H61" t="s" s="2">
         <v>37</v>
@@ -9252,10 +9259,10 @@
         <v>197</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -9285,10 +9292,10 @@
         <v>116</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="Z61" t="s" s="2">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="AA61" t="s" s="2">
         <v>37</v>
@@ -9306,7 +9313,7 @@
         <v>37</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>38</v>
@@ -9315,25 +9322,25 @@
         <v>39</v>
       </c>
       <c r="AI61" t="s" s="2">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="AJ61" t="s" s="2">
         <v>61</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="AM61" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AN61" t="s" s="2">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="AO61" t="s" s="2">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="AP61" t="s" s="2">
         <v>37</v>
@@ -9344,10 +9351,10 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -9361,7 +9368,7 @@
         <v>39</v>
       </c>
       <c r="H62" t="s" s="2">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="I62" t="s" s="2">
         <v>37</v>
@@ -9370,13 +9377,13 @@
         <v>50</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
@@ -9427,7 +9434,7 @@
         <v>37</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>38</v>
@@ -9436,7 +9443,7 @@
         <v>39</v>
       </c>
       <c r="AI62" t="s" s="2">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="AJ62" t="s" s="2">
         <v>61</v>
@@ -9451,24 +9458,24 @@
         <v>37</v>
       </c>
       <c r="AN62" t="s" s="2">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="AO62" t="s" s="2">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="AP62" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AQ62" t="s" s="2">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9482,7 +9489,7 @@
         <v>39</v>
       </c>
       <c r="H63" t="s" s="2">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="I63" t="s" s="2">
         <v>37</v>
@@ -9491,13 +9498,13 @@
         <v>37</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -9548,7 +9555,7 @@
         <v>37</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>38</v>
@@ -9563,16 +9570,16 @@
         <v>61</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="AL63" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="AN63" t="s" s="2">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="AO63" t="s" s="2">
         <v>37</v>
@@ -9581,7 +9588,7 @@
         <v>37</v>
       </c>
       <c r="AQ63" t="s" s="2">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>